<commit_message>
Ajustes em Relartorio de requisitos
</commit_message>
<xml_diff>
--- a/analise/casos de uso/Requisitos de Sistemas.xlsx
+++ b/analise/casos de uso/Requisitos de Sistemas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\TCC\analise\casos de uso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD02B45-E72F-40F0-BB84-4BAFC761DD93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA4B7CF-F98C-420A-B6B9-F5535860833E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,9 +466,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -513,12 +510,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -527,14 +518,23 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -824,7 +824,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A21" sqref="A21:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,439 +862,439 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="12">
-        <v>0</v>
-      </c>
-      <c r="G2" s="13"/>
+      <c r="F2" s="11">
+        <v>0</v>
+      </c>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="14" t="s">
+      <c r="D3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="13"/>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="13"/>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13"/>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="13"/>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13"/>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="14" t="s">
+      <c r="D8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="13"/>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="18" t="s">
+      <c r="D9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13"/>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="22" t="s">
+      <c r="D10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="13"/>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="12">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13"/>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="1:7" ht="95.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="11" t="s">
+      <c r="D12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="13"/>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="30"/>
+      <c r="B13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="D13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="13"/>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="30"/>
+      <c r="B14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="22" t="s">
+      <c r="D14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="12">
-        <v>0</v>
-      </c>
-      <c r="G14" s="13"/>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="22" t="s">
+      <c r="D15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="13"/>
+      <c r="F15" s="11">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="22" t="s">
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="12">
-        <v>0</v>
-      </c>
-      <c r="G16" s="13"/>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="18" t="s">
+      <c r="D17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="12">
-        <v>0</v>
-      </c>
-      <c r="G17" s="13"/>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="11" t="s">
+      <c r="D18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="12">
-        <v>0</v>
-      </c>
-      <c r="G18" s="13"/>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="18" t="s">
+      <c r="D19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="12">
-        <v>0</v>
-      </c>
-      <c r="G19" s="13"/>
+      <c r="F19" s="11">
+        <v>0</v>
+      </c>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="18" t="s">
+      <c r="D20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="12">
-        <v>0</v>
-      </c>
-      <c r="G20" s="13"/>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="24"/>
+      <c r="B21" s="32"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26" t="s">
+      <c r="A22" s="22"/>
+      <c r="B22" s="23" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="26" t="s">
+      <c r="A23" s="24"/>
+      <c r="B23" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="26" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="23" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
+      <c r="A25" s="26"/>
     </row>
     <row r="26" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="31"/>
+      <c r="B26" s="29"/>
     </row>
     <row r="27" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="32">
-        <v>0</v>
-      </c>
-      <c r="B27" s="26" t="s">
+      <c r="A27" s="27">
+        <v>0</v>
+      </c>
+      <c r="B27" s="23" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="32">
+      <c r="A28" s="27">
         <v>1</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="23" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="32">
+      <c r="A29" s="27">
         <v>2</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="23" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A2:A6"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A2:A6"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6">
     <cfRule type="iconSet" priority="15">

</xml_diff>